<commit_message>
readded main method with tweaks
</commit_message>
<xml_diff>
--- a/src/CustomAutoNumber/AN.xlsx
+++ b/src/CustomAutoNumber/AN.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14710" windowHeight="7690"/>
+    <workbookView windowWidth="14710" windowHeight="7280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -329,10 +329,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -369,7 +369,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,11 +390,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -399,55 +406,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +431,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -477,7 +446,22 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -485,14 +469,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,8 +504,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -539,25 +539,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,7 +659,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,19 +683,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,43 +695,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,73 +707,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,26 +793,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -832,17 +832,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,15 +867,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -895,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -913,134 +913,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1060,6 +1060,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1417,7 +1420,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.5"/>
@@ -1497,7 +1500,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
@@ -1600,19 +1603,19 @@
       <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <v>0</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="9">
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -1780,7 +1783,7 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" ht="47.25" spans="1:19">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="4">
@@ -1817,7 +1820,7 @@
       <c r="S10" s="6"/>
     </row>
     <row r="11" ht="31.75" spans="1:19">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B11" s="4">
@@ -1826,14 +1829,14 @@
       <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>51</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="13" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="6" t="s">
@@ -1852,7 +1855,7 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" ht="47.25" spans="1:19">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="4">
@@ -1861,11 +1864,11 @@
       <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G12" s="5"/>
@@ -1876,12 +1879,12 @@
       <c r="J12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="12" t="s">
         <v>57</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="14"/>
+      <c r="N12" s="15"/>
       <c r="O12" s="6" t="s">
         <v>25</v>
       </c>
@@ -1891,7 +1894,7 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" ht="78.25" spans="1:19">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="4">
@@ -1906,7 +1909,7 @@
       <c r="E13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G13" s="6"/>
@@ -1917,12 +1920,12 @@
       <c r="J13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="8" t="s">
         <v>61</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="14"/>
+      <c r="N13" s="15"/>
       <c r="O13" s="6" t="s">
         <v>25</v>
       </c>
@@ -1932,7 +1935,7 @@
       <c r="S13" s="6"/>
     </row>
     <row r="14" ht="78.25" spans="1:19">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="4">
@@ -1947,7 +1950,7 @@
       <c r="E14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G14" s="6"/>
@@ -1958,12 +1961,12 @@
       <c r="J14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="8" t="s">
         <v>64</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="14"/>
+      <c r="N14" s="15"/>
       <c r="O14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="S14" s="6"/>
     </row>
     <row r="15" ht="62.75" spans="1:19">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="4">
@@ -1988,7 +1991,7 @@
       <c r="E15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>55</v>
       </c>
       <c r="G15" s="6"/>
@@ -2002,7 +2005,7 @@
       <c r="K15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="12" t="s">
         <v>68</v>
       </c>
       <c r="M15" s="6"/>
@@ -2016,7 +2019,7 @@
       <c r="S15" s="6"/>
     </row>
     <row r="16" ht="47.25" spans="1:19">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="4">
@@ -2040,18 +2043,18 @@
       <c r="H16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="16" t="s">
         <v>72</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>73</v>
       </c>
       <c r="M16" s="6"/>
-      <c r="N16" s="14"/>
+      <c r="N16" s="15"/>
       <c r="O16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2061,7 +2064,7 @@
       <c r="S16" s="6"/>
     </row>
     <row r="17" ht="62.75" spans="1:19">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="4">
@@ -2070,7 +2073,7 @@
       <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E17" s="6"/>
@@ -2082,7 +2085,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="14"/>
+      <c r="N17" s="15"/>
       <c r="O17" s="6" t="s">
         <v>25</v>
       </c>
@@ -2092,13 +2095,13 @@
       <c r="S17" s="6"/>
     </row>
     <row r="18" ht="47.25" spans="1:19">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="11" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="4">
         <v>7</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>77</v>
       </c>
       <c r="D18" s="6"/>
@@ -2109,7 +2112,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="14"/>
+      <c r="L18" s="15"/>
       <c r="M18" s="6" t="s">
         <v>25</v>
       </c>
@@ -2121,7 +2124,7 @@
       <c r="S18" s="6"/>
     </row>
     <row r="19" ht="47.25" spans="1:19">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="4">
@@ -2130,13 +2133,13 @@
       <c r="C19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="14">
         <v>0</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="14">
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -2146,11 +2149,11 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="14"/>
+      <c r="L19" s="15"/>
       <c r="M19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="16"/>
+      <c r="N19" s="17"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -2158,16 +2161,16 @@
       <c r="S19" s="6"/>
     </row>
     <row r="20" ht="93.75" spans="1:19">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="4">
         <v>7</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>60</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2183,7 +2186,7 @@
         <v>83</v>
       </c>
       <c r="K20" s="6"/>
-      <c r="L20" s="14"/>
+      <c r="L20" s="15"/>
       <c r="M20" s="6" t="s">
         <v>25</v>
       </c>
@@ -2195,13 +2198,13 @@
       <c r="S20" s="6"/>
     </row>
     <row r="21" ht="62.75" spans="1:19">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B21" s="4">
         <v>7</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -2222,7 +2225,7 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="17" t="s">
+      <c r="L21" s="18" t="s">
         <v>60</v>
       </c>
       <c r="M21" s="6" t="s">
@@ -2236,13 +2239,13 @@
       <c r="S21" s="6"/>
     </row>
     <row r="22" ht="78.25" spans="1:19">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B22" s="4">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="6"/>
@@ -2259,7 +2262,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="14"/>
+      <c r="L22" s="15"/>
       <c r="M22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2271,7 +2274,7 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" ht="109.25" spans="1:19">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="4">
@@ -2296,7 +2299,7 @@
         <v>91</v>
       </c>
       <c r="K23" s="6"/>
-      <c r="L23" s="14"/>
+      <c r="L23" s="15"/>
       <c r="M23" s="6" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2311,7 @@
       <c r="S23" s="6"/>
     </row>
     <row r="24" ht="47.25" spans="1:19">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="11" t="s">
         <v>92</v>
       </c>
       <c r="B24" s="4">
@@ -2339,7 +2342,7 @@
       <c r="K24" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="L24" s="14"/>
+      <c r="L24" s="15"/>
       <c r="M24" s="6" t="s">
         <v>25</v>
       </c>
@@ -2351,7 +2354,7 @@
       <c r="S24" s="6"/>
     </row>
     <row r="25" ht="93.75" spans="1:19">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>95</v>
       </c>
       <c r="B25" s="4">
@@ -2374,7 +2377,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="14"/>
+      <c r="L25" s="15"/>
       <c r="M25" s="6" t="s">
         <v>25</v>
       </c>
@@ -2386,7 +2389,7 @@
       <c r="S25" s="6"/>
     </row>
     <row r="26" ht="47.25" spans="1:19">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="11" t="s">
         <v>96</v>
       </c>
       <c r="B26" s="4">
@@ -2407,7 +2410,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="14"/>
+      <c r="L26" s="15"/>
       <c r="M26" s="6" t="s">
         <v>25</v>
       </c>
@@ -2419,7 +2422,7 @@
       <c r="S26" s="6"/>
     </row>
     <row r="27" ht="78.25" spans="1:19">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>98</v>
       </c>
       <c r="B27" s="4">
@@ -2446,7 +2449,7 @@
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="14"/>
+      <c r="L27" s="15"/>
       <c r="M27" s="6" t="s">
         <v>25</v>
       </c>

</xml_diff>